<commit_message>
[feature] Govdocs Select results added.
</commit_message>
<xml_diff>
--- a/benchmark-results/excel-report/all-benchmark-results.xlsx
+++ b/benchmark-results/excel-report/all-benchmark-results.xlsx
@@ -7,18 +7,20 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="547"/>
   </bookViews>
   <sheets>
-    <sheet name="fake_govdocs-analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="fake-govdocs-chart" sheetId="3" r:id="rId2"/>
-    <sheet name="wavs-analysis" sheetId="2" r:id="rId3"/>
-    <sheet name="wavs-analysis-chart" sheetId="4" r:id="rId4"/>
-    <sheet name="wavs-analysis-chart-no-nolimit" sheetId="5" r:id="rId5"/>
+    <sheet name="govdocs-analysis" sheetId="7" r:id="rId1"/>
+    <sheet name="govdocs-chart" sheetId="6" r:id="rId2"/>
+    <sheet name="fake_govdocs-analysis" sheetId="1" r:id="rId3"/>
+    <sheet name="fake-govdocs-chart" sheetId="3" r:id="rId4"/>
+    <sheet name="wavs-analysis" sheetId="2" r:id="rId5"/>
+    <sheet name="wavs-analysis-chart" sheetId="4" r:id="rId6"/>
+    <sheet name="wavs-analysis-chart-no-nolimit" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="60">
   <si>
     <t>Tool Detail</t>
   </si>
@@ -174,6 +176,30 @@
   </si>
   <si>
     <t>sf -sig siegfried.sigs\\no-container\\65535-1.6.2-v86-july2016-nocontainer-default.sig c:\\working\\droid-test\\wavs</t>
+  </si>
+  <si>
+    <t>sha1deep -r c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>md5deep -r c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>sf -sig siegfried.sigs\\container\\NOLIMIT-1.6.2-v86-july2016-default.sig c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>sf -sig siegfried.sigs\\no-container\\NOLIMIT-1.6.2-v86-july2016-nocontainer-default.sig c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>sf -sig siegfried.sigs\\container\\10MB-1.6.2-v86-july2016-default.sig c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>sf -sig siegfried.sigs\\no-container\\10MB-1.6.2-v86-july2016-nocontainer-default.sig c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>sf -sig siegfried.sigs\\container\\65535-1.6.2-v86-july2016-default.sig c:\\working\\droid-test\\govdocs</t>
+  </si>
+  <si>
+    <t>sf -sig siegfried.sigs\\no-container\\65535-1.6.2-v86-july2016-nocontainer-default.sig c:\\working\\droid-test\\govdocs</t>
   </si>
 </sst>
 </file>
@@ -218,13 +244,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +267,333 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="130"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="30"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Time Taken (Minutes)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Govdocs Select</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Corpus</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'govdocs-analysis'!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean Time Taken (Minutes)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'govdocs-analysis'!$P$1:$P$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="15"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.86109999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.54620000000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.95709999999999995</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.6546000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.78720000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.107</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.8200000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.0300000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.6797</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.43769999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.96519999999999995</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0.77</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>9.1999999999999998E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.7999999999999996E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'govdocs-analysis'!$B$2:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>SHA1DEEP 64-bit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MD5DEEP 64-bit</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DROID container NOLIMIT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DROID no-container NOLIMIT</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DROID container 10MB</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DROID no-container 10MB</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DROID container 65535 bytes</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DROID no-container 65535 bytes</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SF container NOLIMIT</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SF no-container NOLIMIT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>SF container 10MB</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>SF no-container 10MB</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SF container 65535 bytes</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>SF no-container 65535 bytes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'govdocs-analysis'!$O$2:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>25.114699999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.3583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.977599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.145399999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.770399999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.631699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.88790000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.80889999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.961300000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.747299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.929200000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.414000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2504</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="162870784"/>
+        <c:axId val="162877440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="162870784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="162877440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="162877440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-NZ" baseline="0"/>
+                  <a:t> Taken (Minutes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-NZ"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="162870784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-NZ"/>
@@ -479,11 +833,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="31120768"/>
-        <c:axId val="202265344"/>
+        <c:axId val="113494272"/>
+        <c:axId val="113537024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31120768"/>
+        <c:axId val="113494272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +846,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202265344"/>
+        <c:crossAx val="113537024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -500,7 +854,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202265344"/>
+        <c:axId val="113537024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,7 +885,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31120768"/>
+        <c:crossAx val="113494272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -554,7 +908,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-NZ"/>
@@ -794,11 +1148,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="201030656"/>
-        <c:axId val="201048832"/>
+        <c:axId val="114616576"/>
+        <c:axId val="114618368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="201030656"/>
+        <c:axId val="114616576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +1161,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201048832"/>
+        <c:crossAx val="114618368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -815,7 +1169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201048832"/>
+        <c:axId val="114618368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +1205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201030656"/>
+        <c:crossAx val="114616576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -874,7 +1228,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-NZ"/>
@@ -1110,11 +1464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="201124864"/>
-        <c:axId val="202572544"/>
+        <c:axId val="114428160"/>
+        <c:axId val="114434048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="201124864"/>
+        <c:axId val="114428160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1123,7 +1477,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="202572544"/>
+        <c:crossAx val="114434048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1131,7 +1485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202572544"/>
+        <c:axId val="114434048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,7 +1521,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201124864"/>
+        <c:crossAx val="114428160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1191,6 +1545,43 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1227,7 +1618,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1264,7 +1655,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1590,8 +1981,798 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="101" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1513.9900000099999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1494.48000002</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1489.1530001199999</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1611.9979999100001</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1585.0309999000001</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1519.0950000299999</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1481.2739999299999</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1468.05899978</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1431.954</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1473.81599998</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1506.885</v>
+      </c>
+      <c r="N2" s="3">
+        <v>51.667200000000001</v>
+      </c>
+      <c r="O2" s="3">
+        <v>25.114699999999999</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0.86109999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1448.05699992</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1422.71200013</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1427.48300004</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1447.0190000499999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1459.796</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1449.26300001</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1477.23199987</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1452.4360001099999</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1489.23699999</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1541.7309999500001</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1461.4965999999999</v>
+      </c>
+      <c r="N3" s="3">
+        <v>32.773099999999999</v>
+      </c>
+      <c r="O3" s="3">
+        <v>24.3583</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.54620000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1523.53299999</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1399.0839998700001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1414.44499993</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1571.7590000600001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1399.0820000199999</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1392.8129999600001</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1422.01600003</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1394.7809999000001</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1435.0410001299999</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1434.0109999199999</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1438.6565000000001</v>
+      </c>
+      <c r="N4" s="3">
+        <v>57.4255</v>
+      </c>
+      <c r="O4" s="3">
+        <v>23.977599999999999</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.95709999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1426.1500000999999</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1384.0299999700001</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1389.28500009</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1224.47099996</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1238.30699992</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1262.56599998</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1215.5030000199999</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1290.2200000299999</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1115.8940000499999</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1140.79099989</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1268.7217000000001</v>
+      </c>
+      <c r="N5" s="3">
+        <v>99.274000000000001</v>
+      </c>
+      <c r="O5" s="3">
+        <v>21.145399999999999</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1.6546000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1239.8990001699999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1108.1099999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1104.6020000000001</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1187.8059999899999</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1118.84200001</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1133.0539999</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1097.01800013</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1090.9179999800001</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1083.3829999</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1098.62000012</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1126.2252000000001</v>
+      </c>
+      <c r="N6" s="3">
+        <v>47.231299999999997</v>
+      </c>
+      <c r="O6" s="3">
+        <v>18.770399999999999</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.78720000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1048.5170002</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1043.6809999899999</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1029.1719999300001</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1190.5090000600001</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1176.5939998599999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1030.34299994</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1008.8900001</v>
+      </c>
+      <c r="J7" s="4">
+        <v>998.06200003599997</v>
+      </c>
+      <c r="K7" s="4">
+        <v>990.375</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1062.8849999900001</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1057.9028000000001</v>
+      </c>
+      <c r="N7" s="3">
+        <v>66.419399999999996</v>
+      </c>
+      <c r="O7" s="3">
+        <v>17.631699999999999</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1.107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4">
+        <v>68.892999887499997</v>
+      </c>
+      <c r="D8" s="4">
+        <v>51.358999967599999</v>
+      </c>
+      <c r="E8" s="4">
+        <v>51.124000072500003</v>
+      </c>
+      <c r="F8" s="4">
+        <v>52.138999939000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>51.108999967599999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>53.620000124000001</v>
+      </c>
+      <c r="I8" s="4">
+        <v>50.641000032400001</v>
+      </c>
+      <c r="J8" s="4">
+        <v>52.185999870300002</v>
+      </c>
+      <c r="K8" s="4">
+        <v>49.937999963800003</v>
+      </c>
+      <c r="L8" s="4">
+        <v>51.702000141100001</v>
+      </c>
+      <c r="M8" s="3">
+        <v>53.271099999999997</v>
+      </c>
+      <c r="N8" s="3">
+        <v>5.2919999999999998</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.88790000000000002</v>
+      </c>
+      <c r="P8" s="3">
+        <v>8.8200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4">
+        <v>52.638000011400003</v>
+      </c>
+      <c r="D9" s="4">
+        <v>45.898999929399999</v>
+      </c>
+      <c r="E9" s="4">
+        <v>45.944999933200002</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45.2120001316</v>
+      </c>
+      <c r="G9" s="4">
+        <v>49.5639998913</v>
+      </c>
+      <c r="H9" s="4">
+        <v>46.617000103000002</v>
+      </c>
+      <c r="I9" s="4">
+        <v>51.7789998055</v>
+      </c>
+      <c r="J9" s="4">
+        <v>48.878000020999998</v>
+      </c>
+      <c r="K9" s="4">
+        <v>49.657999992400001</v>
+      </c>
+      <c r="L9" s="4">
+        <v>49.128000020999998</v>
+      </c>
+      <c r="M9" s="3">
+        <v>48.531799999999997</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2.4192</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.80889999999999995</v>
+      </c>
+      <c r="P9" s="3">
+        <v>4.0300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4">
+        <v>925.00800013499997</v>
+      </c>
+      <c r="D10" s="4">
+        <v>917.37900018699997</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1211.7610001600001</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1113.94199991</v>
+      </c>
+      <c r="G10" s="4">
+        <v>937.19199991200003</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1122.0060000399999</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1091.94499993</v>
+      </c>
+      <c r="J10" s="4">
+        <v>964.41400003399997</v>
+      </c>
+      <c r="K10" s="4">
+        <v>937.64400005300001</v>
+      </c>
+      <c r="L10" s="4">
+        <v>955.45899987200005</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1017.675</v>
+      </c>
+      <c r="N10" s="3">
+        <v>100.78400000000001</v>
+      </c>
+      <c r="O10" s="3">
+        <v>16.961300000000001</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1.6797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1081.44499993</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1099.33899999</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1048.8109998699999</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1044.76899981</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1030.44899988</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1034.8489999799999</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1049.125</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1060.9369998</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1094.5030000199999</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1104.17500019</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1064.8402000000001</v>
+      </c>
+      <c r="N11" s="3">
+        <v>26.262499999999999</v>
+      </c>
+      <c r="O11" s="3">
+        <v>17.747299999999999</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.43769999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1013.102</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1008.71799994</v>
+      </c>
+      <c r="E12" s="4">
+        <v>981.978999853</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1041.10399985</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1145.5</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1082.41300011</v>
+      </c>
+      <c r="I12" s="4">
+        <v>958.00300002100005</v>
+      </c>
+      <c r="J12" s="4">
+        <v>951.55999994299998</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1013.75699997</v>
+      </c>
+      <c r="L12" s="4">
+        <v>961.37199997899995</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1015.7508</v>
+      </c>
+      <c r="N12" s="3">
+        <v>57.909199999999998</v>
+      </c>
+      <c r="O12" s="3">
+        <v>16.929200000000002</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.96519999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1017.59699988</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1020.56399989</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1012.602</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1017.36100006</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1027.625</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1015.03600001</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1170.28799987</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1059.34099984</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1032.5399999599999</v>
+      </c>
+      <c r="L13" s="4">
+        <v>1075.42400002</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1044.8378</v>
+      </c>
+      <c r="N13" s="3">
+        <v>46.200299999999999</v>
+      </c>
+      <c r="O13" s="3">
+        <v>17.414000000000001</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4">
+        <v>76.628000021000005</v>
+      </c>
+      <c r="D14" s="4">
+        <v>74.957999944700006</v>
+      </c>
+      <c r="E14" s="4">
+        <v>74.724999904599997</v>
+      </c>
+      <c r="F14" s="4">
+        <v>74.661999940900003</v>
+      </c>
+      <c r="G14" s="4">
+        <v>74.9270000458</v>
+      </c>
+      <c r="H14" s="4">
+        <v>74.693000078200001</v>
+      </c>
+      <c r="I14" s="4">
+        <v>74.990000009499994</v>
+      </c>
+      <c r="J14" s="4">
+        <v>75.144999980899996</v>
+      </c>
+      <c r="K14" s="4">
+        <v>74.772000074399998</v>
+      </c>
+      <c r="L14" s="4">
+        <v>74.756000041999997</v>
+      </c>
+      <c r="M14" s="3">
+        <v>75.025599999999997</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.55389999999999995</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1.2504</v>
+      </c>
+      <c r="P14" s="3">
+        <v>9.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="4">
+        <v>78.514999866500006</v>
+      </c>
+      <c r="D15" s="4">
+        <v>78.296999931299993</v>
+      </c>
+      <c r="E15" s="4">
+        <v>78.328000068700007</v>
+      </c>
+      <c r="F15" s="4">
+        <v>78.531000137299998</v>
+      </c>
+      <c r="G15" s="4">
+        <v>78.453000068700007</v>
+      </c>
+      <c r="H15" s="4">
+        <v>78.048000097300005</v>
+      </c>
+      <c r="I15" s="4">
+        <v>78.141000032400001</v>
+      </c>
+      <c r="J15" s="4">
+        <v>79.093000173600004</v>
+      </c>
+      <c r="K15" s="4">
+        <v>78.094000101099994</v>
+      </c>
+      <c r="L15" s="4">
+        <v>78.265000104899997</v>
+      </c>
+      <c r="M15" s="3">
+        <v>78.376499999999993</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="O15" s="3">
+        <v>1.3063</v>
+      </c>
+      <c r="P15" s="3">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2366,7 +3547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2381,7 +3562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
@@ -3157,7 +4338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3172,7 +4353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>